<commit_message>
Deleted Eagle Buck schematic
Replaced by Altium design instead.
</commit_message>
<xml_diff>
--- a/Documentos/Buck.xlsx
+++ b/Documentos/Buck.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ef58da02b93602f7/ITESM/GrupoInvestigacion/Converters/Documentos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tec de Monterrey\Power Electronics Gerardo Escobar\Simple Boost Converter\Simple_Boost_Converter\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="799" documentId="11_F4FDDCD2CDE8D03A7F0AB384521CA8AB9A5333FD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E98F1BCD-6D15-4D8B-98BC-27EBD390574A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD96534-9A1B-4C53-85B3-2129EC75D6E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Buck" sheetId="4" r:id="rId1"/>
@@ -375,7 +375,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -392,7 +392,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -694,7 +694,7 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="55.33203125" customWidth="1"/>
     <col min="4" max="4" width="14.44140625" customWidth="1"/>

</xml_diff>